<commit_message>
Added few more featrures in the excel file
</commit_message>
<xml_diff>
--- a/src/main/java/com/qa/testdata/TestDataDriven.xlsx
+++ b/src/main/java/com/qa/testdata/TestDataDriven.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Selenium\eclipse-workspace1\DataDrivenFrameWork\src\main\java\com\qa\testdata\"/>
     </mc:Choice>
@@ -13,10 +13,12 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" r:id="rId5" sheetId="2"/>
+    <sheet name="Homepage" r:id="rId6" sheetId="3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -87,7 +89,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -432,9 +435,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -521,4 +524,28 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId9"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added the Webtable Handling
</commit_message>
<xml_diff>
--- a/src/main/java/com/qa/testdata/TestDataDriven.xlsx
+++ b/src/main/java/com/qa/testdata/TestDataDriven.xlsx
@@ -15,6 +15,9 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" r:id="rId5" sheetId="2"/>
     <sheet name="Homepage" r:id="rId6" sheetId="3"/>
+    <sheet name="Webtable" r:id="rId7" sheetId="4"/>
+    <sheet name="Webtable2" r:id="rId8" sheetId="5"/>
+    <sheet name="Webtable3" r:id="rId9" sheetId="6"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="40">
   <si>
     <t>firstname</t>
   </si>
@@ -83,6 +86,69 @@
   </si>
   <si>
     <t>Rainingsrh@1011</t>
+  </si>
+  <si>
+    <t>Company</t>
+  </si>
+  <si>
+    <t>Contact</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>Alfreds Futterkiste</t>
+  </si>
+  <si>
+    <t>Maria Anders</t>
+  </si>
+  <si>
+    <t>Germany</t>
+  </si>
+  <si>
+    <t>Centro comercial Moctezuma</t>
+  </si>
+  <si>
+    <t>Francisco Chang</t>
+  </si>
+  <si>
+    <t>Mexico</t>
+  </si>
+  <si>
+    <t>Ernst Handel</t>
+  </si>
+  <si>
+    <t>Roland Mendel</t>
+  </si>
+  <si>
+    <t>Austria</t>
+  </si>
+  <si>
+    <t>Island Trading</t>
+  </si>
+  <si>
+    <t>Helen Bennett</t>
+  </si>
+  <si>
+    <t>UK</t>
+  </si>
+  <si>
+    <t>Laughing Bacchus Winecellars</t>
+  </si>
+  <si>
+    <t>Yoshi Tannamuri</t>
+  </si>
+  <si>
+    <t>Canada</t>
+  </si>
+  <si>
+    <t>Magazzini Alimentari Riuniti</t>
+  </si>
+  <si>
+    <t>Giovanni Rovelli</t>
+  </si>
+  <si>
+    <t>Italy</t>
   </si>
 </sst>
 </file>
@@ -115,7 +181,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="81">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -126,6 +192,396 @@
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
       </patternFill>
     </fill>
   </fills>
@@ -142,10 +598,49 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="30" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="32" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="40" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="42" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="44" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="46" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="48" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="50" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="52" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="54" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="56" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="58" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="60" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="62" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="64" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="66" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="68" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="70" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="72" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="74" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="76" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="78" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="80" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -548,4 +1043,409 @@
   <sheetData/>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="9.3828125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="7.87890625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="7.83984375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="9.3828125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="7.87890625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="7.83984375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="9.3828125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="7.87890625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="7.83984375" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="9.3828125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="7.87890625" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="7.83984375" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="9.3828125" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="7.87890625" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="7.83984375" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="9.3828125" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="7.87890625" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="7.83984375" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s" s="3">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s" s="4">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s" s="5">
+        <v>21</v>
+      </c>
+      <c r="D1" t="s" s="6">
+        <v>19</v>
+      </c>
+      <c r="E1" t="s" s="7">
+        <v>20</v>
+      </c>
+      <c r="F1" t="s" s="8">
+        <v>21</v>
+      </c>
+      <c r="G1" t="s" s="9">
+        <v>19</v>
+      </c>
+      <c r="H1" t="s" s="10">
+        <v>20</v>
+      </c>
+      <c r="I1" t="s" s="11">
+        <v>21</v>
+      </c>
+      <c r="J1" t="s" s="12">
+        <v>19</v>
+      </c>
+      <c r="K1" t="s" s="13">
+        <v>20</v>
+      </c>
+      <c r="L1" t="s" s="14">
+        <v>21</v>
+      </c>
+      <c r="M1" t="s" s="15">
+        <v>19</v>
+      </c>
+      <c r="N1" t="s" s="16">
+        <v>20</v>
+      </c>
+      <c r="O1" t="s" s="17">
+        <v>21</v>
+      </c>
+      <c r="P1" t="s" s="18">
+        <v>19</v>
+      </c>
+      <c r="Q1" t="s" s="19">
+        <v>20</v>
+      </c>
+      <c r="R1" t="s" s="20">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="D3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="G4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="J5" t="s">
+        <v>31</v>
+      </c>
+      <c r="K5" t="s">
+        <v>32</v>
+      </c>
+      <c r="L5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="M6" t="s">
+        <v>34</v>
+      </c>
+      <c r="N6" t="s">
+        <v>35</v>
+      </c>
+      <c r="O6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="P7" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>38</v>
+      </c>
+      <c r="R7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="9.3828125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="7.87890625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="7.83984375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="9.3828125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="7.87890625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="7.83984375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="9.3828125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="7.87890625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="7.83984375" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="9.3828125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="7.87890625" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="7.83984375" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="9.3828125" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="7.87890625" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="7.83984375" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="9.3828125" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="7.87890625" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="7.83984375" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s" s="21">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s" s="22">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s" s="23">
+        <v>21</v>
+      </c>
+      <c r="D1" t="s" s="24">
+        <v>19</v>
+      </c>
+      <c r="E1" t="s" s="25">
+        <v>20</v>
+      </c>
+      <c r="F1" t="s" s="26">
+        <v>21</v>
+      </c>
+      <c r="G1" t="s" s="27">
+        <v>19</v>
+      </c>
+      <c r="H1" t="s" s="28">
+        <v>20</v>
+      </c>
+      <c r="I1" t="s" s="29">
+        <v>21</v>
+      </c>
+      <c r="J1" t="s" s="30">
+        <v>19</v>
+      </c>
+      <c r="K1" t="s" s="31">
+        <v>20</v>
+      </c>
+      <c r="L1" t="s" s="32">
+        <v>21</v>
+      </c>
+      <c r="M1" t="s" s="33">
+        <v>19</v>
+      </c>
+      <c r="N1" t="s" s="34">
+        <v>20</v>
+      </c>
+      <c r="O1" t="s" s="35">
+        <v>21</v>
+      </c>
+      <c r="P1" t="s" s="36">
+        <v>19</v>
+      </c>
+      <c r="Q1" t="s" s="37">
+        <v>20</v>
+      </c>
+      <c r="R1" t="s" s="38">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="D3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="G4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="J5" t="s">
+        <v>31</v>
+      </c>
+      <c r="K5" t="s">
+        <v>32</v>
+      </c>
+      <c r="L5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="M6" t="s">
+        <v>34</v>
+      </c>
+      <c r="N6" t="s">
+        <v>35</v>
+      </c>
+      <c r="O6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="P7" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>38</v>
+      </c>
+      <c r="R7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="27.578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="15.93359375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="9.15234375" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s" s="39">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s" s="40">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s" s="41">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
 </file>
</xml_diff>